<commit_message>
se añade afinacion. Solo implementado DO=13, la nota numero 13
</commit_message>
<xml_diff>
--- a/notasmusicales.xlsx
+++ b/notasmusicales.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49622986-0C66-44D8-B788-7199A8AA619D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9AE3B7-D306-4B6F-90C0-8AB4B7F4774C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="225">
   <si>
     <t>C</t>
   </si>
@@ -957,9 +957,6 @@
     <t>indice</t>
   </si>
   <si>
-    <t>palabra</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
@@ -985,6 +982,15 @@
   </si>
   <si>
     <t>RE b</t>
+  </si>
+  <si>
+    <t>digitacionDO</t>
+  </si>
+  <si>
+    <t>digitacionSIb</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -1554,703 +1560,736 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BQ66"/>
+  <dimension ref="A1:BR66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A64"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66:BT66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="70" width="1.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="69.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="71" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="25.5" thickBot="1">
+    <row r="1" spans="1:23" ht="25.5" thickBot="1">
       <c r="A1" s="8" t="s">
         <v>212</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="E1" s="8"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="8"/>
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="2" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="7">
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="str">
-        <f>CONCATENATE("var ",C2,"=",D2,";")</f>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F33" si="0">CONCATENATE("var ",D2,"=",E2,";")</f>
         <v>var C1=32.70;</v>
       </c>
-      <c r="F2" t="str">
-        <f>CONCATENATE("case '",C2,"': frequency= ",D2,";break;",)</f>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="1">CONCATENATE("case '",D2,"': frequency= ",E2,";break;",)</f>
         <v>case 'C1': frequency= 32.70;break;</v>
       </c>
-      <c r="G2" t="str">
-        <f>CONCATENATE("{",$A$1,": ",A2,",",$B$1,": '",B2,"',",$C$1,": '",C2,"',",$D$1,": ",D2,"}")</f>
-        <v>{indice: 1,palabra: 'DO 0',tipo: 'C1',frecuencia: 32.70}</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" t="str">
+        <f>CONCATENATE("{",$A$1,": ",A2,",",$B$1,": '",B2,"',",$C$1,": '",C2,"',",$D$1,": '",D2,"',",$E$1,": ",E2,"}")</f>
+        <v>{indice: 1,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C1',frecuencia: 32.70}</v>
+      </c>
+      <c r="J2" s="1">
         <v>0</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="7">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="str">
-        <f>CONCATENATE("var ",C3,"=",D3,";")</f>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
         <v>var Cs1=34.65;</v>
       </c>
-      <c r="F3" t="str">
-        <f>CONCATENATE("case '",C3,"': frequency= ",D3,";break;",)</f>
+      <c r="G3" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Cs1': frequency= 34.65;break;</v>
       </c>
-      <c r="G3" t="str">
-        <f t="shared" ref="G3:G64" si="0">CONCATENATE("{",$A$1,": ",A3,",",$B$1,": '",B3,"',",$C$1,": '",C3,"',",$D$1,": ",D3,"}")</f>
-        <v>{indice: 2,palabra: 'C#1',tipo: 'Cs1',frecuencia: 34.65}</v>
-      </c>
-      <c r="I3" s="1">
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:H64" si="2">CONCATENATE("{",$A$1,": ",A3,",",$B$1,": '",B3,"',",$C$1,": '",C3,"',",$D$1,": '",D3,"',",$E$1,": ",E3,"}")</f>
+        <v>{indice: 2,digitacionDO: 'C#1',digitacionSIb: '?',tipo: 'Cs1',frecuencia: 34.65}</v>
+      </c>
+      <c r="J3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="4" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A4" s="7">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="str">
-        <f>CONCATENATE("var ",C4,"=",D4,";")</f>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
         <v>var D1=36.71;</v>
       </c>
-      <c r="F4" t="str">
-        <f>CONCATENATE("case '",C4,"': frequency= ",D4,";break;",)</f>
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
         <v>case 'D1': frequency= 36.71;break;</v>
       </c>
-      <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 3,palabra: 'D1',tipo: 'D1',frecuencia: 36.71}</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 3,digitacionDO: 'D1',digitacionSIb: '?',tipo: 'D1',frecuencia: 36.71}</v>
+      </c>
+      <c r="J4" s="1">
         <v>2</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="P4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="R4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="5" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A5" s="7">
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="str">
-        <f>CONCATENATE("var ",C5,"=",D5,";")</f>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
         <v>var Eb1=38.89;</v>
       </c>
-      <c r="F5" t="str">
-        <f>CONCATENATE("case '",C5,"': frequency= ",D5,";break;",)</f>
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Eb1': frequency= 38.89;break;</v>
       </c>
-      <c r="G5" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 4,palabra: 'Eb1',tipo: 'Eb1',frecuencia: 38.89}</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 4,digitacionDO: 'Eb1',digitacionSIb: '?',tipo: 'Eb1',frecuencia: 38.89}</v>
+      </c>
+      <c r="J5" s="1">
         <v>3</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1"/>
+      <c r="L5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="P5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="R5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="S5" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="U5" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="6" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A6" s="7">
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" t="str">
-        <f>CONCATENATE("var ",C6,"=",D6,";")</f>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
         <v>var E1=41.20;</v>
       </c>
-      <c r="F6" t="str">
-        <f>CONCATENATE("case '",C6,"': frequency= ",D6,";break;",)</f>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
         <v>case 'E1': frequency= 41.20;break;</v>
       </c>
-      <c r="G6" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 5,palabra: 'E1',tipo: 'E1',frecuencia: 41.20}</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 5,digitacionDO: 'E1',digitacionSIb: '?',tipo: 'E1',frecuencia: 41.20}</v>
+      </c>
+      <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1"/>
+      <c r="L6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="P6" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="S6" s="2" t="s">
+      <c r="T6" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U6" s="2" t="s">
+      <c r="V6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="V6" s="2" t="s">
+      <c r="W6" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="7" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A7" s="7">
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" t="str">
-        <f>CONCATENATE("var ",C7,"=",D7,";")</f>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
         <v>var F1=43.65;</v>
       </c>
-      <c r="F7" t="str">
-        <f>CONCATENATE("case '",C7,"': frequency= ",D7,";break;",)</f>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
         <v>case 'F1': frequency= 43.65;break;</v>
       </c>
-      <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 6,palabra: 'F1',tipo: 'F1',frecuencia: 43.65}</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 6,digitacionDO: 'F1',digitacionSIb: '?',tipo: 'F1',frecuencia: 43.65}</v>
+      </c>
+      <c r="J7" s="1">
         <v>5</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" thickBot="1">
+    <row r="8" spans="1:23" ht="15" customHeight="1" thickBot="1">
       <c r="A8" s="7">
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" t="str">
-        <f>CONCATENATE("var ",C8,"=",D8,";")</f>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
         <v>var Fs1=46.25;</v>
       </c>
-      <c r="F8" t="str">
-        <f>CONCATENATE("case '",C8,"': frequency= ",D8,";break;",)</f>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Fs1': frequency= 46.25;break;</v>
       </c>
-      <c r="G8" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 7,palabra: 'F#1',tipo: 'Fs1',frecuencia: 46.25}</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 7,digitacionDO: 'F#1',digitacionSIb: '?',tipo: 'Fs1',frecuencia: 46.25}</v>
+      </c>
+      <c r="J8" s="1">
         <v>6</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="2">
+      <c r="K8" s="1"/>
+      <c r="L8" s="2">
         <v>1047</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>1109</v>
       </c>
-      <c r="M8" s="2">
+      <c r="N8" s="2">
         <v>1175</v>
       </c>
-      <c r="N8" s="2">
+      <c r="O8" s="2">
         <v>1245</v>
       </c>
-      <c r="O8" s="2">
+      <c r="P8" s="2">
         <v>1319</v>
       </c>
-      <c r="P8" s="2">
+      <c r="Q8" s="2">
         <v>1397</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>1480</v>
       </c>
-      <c r="R8" s="2">
+      <c r="S8" s="2">
         <v>1568</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>1661</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>1760</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>1865</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
         <v>1976</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15.75" thickBot="1">
+    <row r="9" spans="1:23" ht="15.75" thickBot="1">
       <c r="A9" s="7">
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="str">
-        <f>CONCATENATE("var ",C9,"=",D9,";")</f>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
         <v>var G1=49.00;</v>
       </c>
-      <c r="F9" t="str">
-        <f>CONCATENATE("case '",C9,"': frequency= ",D9,";break;",)</f>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
         <v>case 'G1': frequency= 49.00;break;</v>
       </c>
-      <c r="G9" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 8,palabra: 'G1',tipo: 'G1',frecuencia: 49.00}</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 8,digitacionDO: 'G1',digitacionSIb: '?',tipo: 'G1',frecuencia: 49.00}</v>
+      </c>
+      <c r="J9" s="1">
         <v>7</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2">
+      <c r="K9" s="1"/>
+      <c r="L9" s="2">
         <v>2093</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>2217</v>
       </c>
-      <c r="M9" s="2">
+      <c r="N9" s="2">
         <v>2349</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>2489</v>
       </c>
-      <c r="O9" s="2">
+      <c r="P9" s="2">
         <v>2637</v>
       </c>
-      <c r="P9" s="2">
+      <c r="Q9" s="2">
         <v>2794</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>2960</v>
       </c>
-      <c r="R9" s="2">
+      <c r="S9" s="2">
         <v>3136</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>3322</v>
       </c>
-      <c r="T9" s="2">
+      <c r="U9" s="2">
         <v>3520</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>3729</v>
       </c>
-      <c r="V9" s="2">
+      <c r="W9" s="2">
         <v>3951</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1">
+    <row r="10" spans="1:23" ht="15.75" thickBot="1">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="str">
-        <f>CONCATENATE("var ",C10,"=",D10,";")</f>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
         <v>var Gs1=51.91;</v>
       </c>
-      <c r="F10" t="str">
-        <f>CONCATENATE("case '",C10,"': frequency= ",D10,";break;",)</f>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Gs1': frequency= 51.91;break;</v>
       </c>
-      <c r="G10" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 9,palabra: 'G#1',tipo: 'Gs1',frecuencia: 51.91}</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 9,digitacionDO: 'G#1',digitacionSIb: '?',tipo: 'Gs1',frecuencia: 51.91}</v>
+      </c>
+      <c r="J10" s="1">
         <v>8</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="2">
+      <c r="K10" s="1"/>
+      <c r="L10" s="2">
         <v>4186</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>4435</v>
       </c>
-      <c r="M10" s="2">
+      <c r="N10" s="2">
         <v>4699</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>4978</v>
       </c>
-      <c r="O10" s="2">
+      <c r="P10" s="2">
         <v>5274</v>
       </c>
-      <c r="P10" s="2">
+      <c r="Q10" s="2">
         <v>5588</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>5920</v>
       </c>
-      <c r="R10" s="2">
+      <c r="S10" s="2">
         <v>6272</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>6645</v>
       </c>
-      <c r="T10" s="2">
+      <c r="U10" s="2">
         <v>7040</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>7459</v>
       </c>
-      <c r="V10" s="2">
+      <c r="W10" s="2">
         <v>7902</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="15.75" thickBot="1">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D11" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E11" t="str">
-        <f>CONCATENATE("var ",C11,"=",D11,";")</f>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
         <v>var A1=55.00;</v>
       </c>
-      <c r="F11" t="str">
-        <f>CONCATENATE("case '",C11,"': frequency= ",D11,";break;",)</f>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
         <v>case 'A1': frequency= 55.00;break;</v>
       </c>
-      <c r="G11" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 10,palabra: 'LA 1-2',tipo: 'A1',frecuencia: 55.00}</v>
-      </c>
-      <c r="I11" s="4"/>
+      <c r="H11" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 10,digitacionDO: 'LA 1-2',digitacionSIb: '?',tipo: 'A1',frecuencia: 55.00}</v>
+      </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
+      <c r="K11" s="4"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
@@ -2262,1582 +2301,1744 @@
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
       <c r="V11" s="5"/>
-    </row>
-    <row r="12" spans="1:22" ht="15.75" thickBot="1">
+      <c r="W11" s="5"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickBot="1">
       <c r="A12" s="7">
         <v>11</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="str">
-        <f>CONCATENATE("var ",C12,"=",D12,";")</f>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
         <v>var Bb1=58.27;</v>
       </c>
-      <c r="F12" t="str">
-        <f>CONCATENATE("case '",C12,"': frequency= ",D12,";break;",)</f>
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Bb1': frequency= 58.27;break;</v>
       </c>
-      <c r="G12" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 11,palabra: 'SIb 1',tipo: 'Bb1',frecuencia: 58.27}</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" ht="15.75" thickBot="1">
+      <c r="H12" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 11,digitacionDO: 'SIb 1',digitacionSIb: '?',tipo: 'Bb1',frecuencia: 58.27}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" thickBot="1">
       <c r="A13" s="7">
         <v>12</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E13" t="str">
-        <f>CONCATENATE("var ",C13,"=",D13,";")</f>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
         <v>var B1=61.74;</v>
       </c>
-      <c r="F13" t="str">
-        <f>CONCATENATE("case '",C13,"': frequency= ",D13,";break;",)</f>
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
         <v>case 'B1': frequency= 61.74;break;</v>
       </c>
-      <c r="G13" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 12,palabra: 'SI 2',tipo: 'B1',frecuencia: 61.74}</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="15.75" thickBot="1">
+      <c r="H13" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 12,digitacionDO: 'SI 2',digitacionSIb: '?',tipo: 'B1',frecuencia: 61.74}</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1">
       <c r="A14" s="7">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="str">
-        <f>CONCATENATE("var ",C14,"=",D14,";")</f>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
         <v>var C2=65.41;</v>
       </c>
-      <c r="F14" t="str">
-        <f>CONCATENATE("case '",C14,"': frequency= ",D14,";break;",)</f>
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
         <v>case 'C2': frequency= 65.41;break;</v>
       </c>
-      <c r="G14" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 13,palabra: 'DO 0',tipo: 'C2',frecuencia: 65.41}</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="15.75" thickBot="1">
+      <c r="H14" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 13,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C2',frecuencia: 65.41}</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15.75" thickBot="1">
       <c r="A15" s="7">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C15" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E15" t="str">
-        <f>CONCATENATE("var ",C15,"=",D15,";")</f>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
         <v>var Cs2=69.30;</v>
       </c>
-      <c r="F15" t="str">
-        <f>CONCATENATE("case '",C15,"': frequency= ",D15,";break;",)</f>
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Cs2': frequency= 69.30;break;</v>
       </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 14,palabra: 'DO#',tipo: 'Cs2',frecuencia: 69.30}</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="15.75" thickBot="1">
+      <c r="H15" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 14,digitacionDO: 'DO#',digitacionSIb: '?',tipo: 'Cs2',frecuencia: 69.30}</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" thickBot="1">
       <c r="A16" s="7">
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="C16" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E16" t="str">
-        <f>CONCATENATE("var ",C16,"=",D16,";")</f>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
         <v>var Db2=69.30;</v>
       </c>
-      <c r="F16" t="str">
-        <f>CONCATENATE("case '",C16,"': frequency= ",D16,";break;",)</f>
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Db2': frequency= 69.30;break;</v>
       </c>
-      <c r="G16" t="str">
-        <f t="shared" ref="G16" si="1">CONCATENATE("{",$A$1,": ",A16,",",$B$1,": '",B16,"',",$C$1,": '",C16,"',",$D$1,": ",D16,"}")</f>
-        <v>{indice: 15,palabra: 'RE b',tipo: 'Db2',frecuencia: 69.30}</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H16" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 15,digitacionDO: 'RE b',digitacionSIb: '?',tipo: 'Db2',frecuencia: 69.30}</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="7">
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C17" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E17" t="str">
-        <f>CONCATENATE("var ",C17,"=",D17,";")</f>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
         <v>var D2=73.42;</v>
       </c>
-      <c r="F17" t="str">
-        <f>CONCATENATE("case '",C17,"': frequency= ",D17,";break;",)</f>
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
         <v>case 'D2': frequency= 73.42;break;</v>
       </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 16,palabra: 'RE',tipo: 'D2',frecuencia: 73.42}</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H17" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 16,digitacionDO: 'RE',digitacionSIb: '?',tipo: 'D2',frecuencia: 73.42}</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1">
       <c r="A18" s="7">
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="str">
-        <f>CONCATENATE("var ",C18,"=",D18,";")</f>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
         <v>var Ds2=77.78;</v>
       </c>
-      <c r="F18" t="str">
-        <f>CONCATENATE("case '",C18,"': frequency= ",D18,";break;",)</f>
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Ds2': frequency= 77.78;break;</v>
       </c>
-      <c r="G18" t="str">
-        <f t="shared" ref="G18" si="2">CONCATENATE("{",$A$1,": ",A18,",",$B$1,": '",B18,"',",$C$1,": '",C18,"',",$D$1,": ",D18,"}")</f>
-        <v>{indice: 17,palabra: 'RE#',tipo: 'Ds2',frecuencia: 77.78}</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H18" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 17,digitacionDO: 'RE#',digitacionSIb: '?',tipo: 'Ds2',frecuencia: 77.78}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1">
       <c r="A19" s="7">
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="C19" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D19" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" t="str">
-        <f>CONCATENATE("var ",C19,"=",D19,";")</f>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
         <v>var Eb2=77.78;</v>
       </c>
-      <c r="F19" t="str">
-        <f>CONCATENATE("case '",C19,"': frequency= ",D19,";break;",)</f>
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Eb2': frequency= 77.78;break;</v>
       </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 18,palabra: 'MI b',tipo: 'Eb2',frecuencia: 77.78}</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H19" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 18,digitacionDO: 'MI b',digitacionSIb: '?',tipo: 'Eb2',frecuencia: 77.78}</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1">
       <c r="A20" s="7">
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C20" s="14" t="s">
+        <v>218</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E20" t="str">
-        <f>CONCATENATE("var ",C20,"=",D20,";")</f>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
         <v>var E2=82.41;</v>
       </c>
-      <c r="F20" t="str">
-        <f>CONCATENATE("case '",C20,"': frequency= ",D20,";break;",)</f>
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
         <v>case 'E2': frequency= 82.41;break;</v>
       </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 19,palabra: 'MI  1-2',tipo: 'E2',frecuencia: 82.41}</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H20" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 19,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E2',frecuencia: 82.41}</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1">
       <c r="A21" s="7">
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E21" t="str">
-        <f>CONCATENATE("var ",C21,"=",D21,";")</f>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
         <v>var F2=87.31;</v>
       </c>
-      <c r="F21" t="str">
-        <f>CONCATENATE("case '",C21,"': frequency= ",D21,";break;",)</f>
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
         <v>case 'F2': frequency= 87.31;break;</v>
       </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 20,palabra: 'FA 1',tipo: 'F2',frecuencia: 87.31}</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H21" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 20,digitacionDO: 'FA 1',digitacionSIb: '?',tipo: 'F2',frecuencia: 87.31}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E22" t="str">
-        <f>CONCATENATE("var ",C22,"=",D22,";")</f>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
         <v>var Fs2=92.50;</v>
       </c>
-      <c r="F22" t="str">
-        <f>CONCATENATE("case '",C22,"': frequency= ",D22,";break;",)</f>
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Fs2': frequency= 92.50;break;</v>
       </c>
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 21,palabra: 'FA# 2',tipo: 'Fs2',frecuencia: 92.50}</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H22" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 21,digitacionDO: 'FA# 2',digitacionSIb: '?',tipo: 'Fs2',frecuencia: 92.50}</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1">
       <c r="A23" s="7">
         <v>22</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="str">
-        <f>CONCATENATE("var ",C23,"=",D23,";")</f>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
         <v>var G2=98.00;</v>
       </c>
-      <c r="F23" t="str">
-        <f>CONCATENATE("case '",C23,"': frequency= ",D23,";break;",)</f>
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
         <v>case 'G2': frequency= 98.00;break;</v>
       </c>
-      <c r="G23" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 22,palabra: 'SOL 0',tipo: 'G2',frecuencia: 98.00}</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H23" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 22,digitacionDO: 'SOL 0',digitacionSIb: '?',tipo: 'G2',frecuencia: 98.00}</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1">
       <c r="A24" s="7">
         <v>23</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="C24" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E24" t="str">
-        <f>CONCATENATE("var ",C24,"=",D24,";")</f>
+      <c r="F24" t="str">
+        <f t="shared" si="0"/>
         <v>var Gs2=103.8;</v>
       </c>
-      <c r="F24" t="str">
-        <f>CONCATENATE("case '",C24,"': frequency= ",D24,";break;",)</f>
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Gs2': frequency= 103.8;break;</v>
       </c>
-      <c r="G24" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 23,palabra: 'SOL#',tipo: 'Gs2',frecuencia: 103.8}</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H24" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 23,digitacionDO: 'SOL#',digitacionSIb: '?',tipo: 'Gs2',frecuencia: 103.8}</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1">
       <c r="A25" s="7">
         <v>24</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="str">
-        <f>CONCATENATE("var ",C25,"=",D25,";")</f>
+      <c r="F25" t="str">
+        <f t="shared" si="0"/>
         <v>var A2=110.0;</v>
       </c>
-      <c r="F25" t="str">
-        <f>CONCATENATE("case '",C25,"': frequency= ",D25,";break;",)</f>
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
         <v>case 'A2': frequency= 110.0;break;</v>
       </c>
-      <c r="G25" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 24,palabra: 'LA 1-2',tipo: 'A2',frecuencia: 110.0}</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H25" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 24,digitacionDO: 'LA 1-2',digitacionSIb: '?',tipo: 'A2',frecuencia: 110.0}</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1">
       <c r="A26" s="7">
         <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E26" t="str">
-        <f>CONCATENATE("var ",C26,"=",D26,";")</f>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
         <v>var Bb2=116.5;</v>
       </c>
-      <c r="F26" t="str">
-        <f>CONCATENATE("case '",C26,"': frequency= ",D26,";break;",)</f>
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Bb2': frequency= 116.5;break;</v>
       </c>
-      <c r="G26" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 25,palabra: 'SIb 1',tipo: 'Bb2',frecuencia: 116.5}</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H26" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 25,digitacionDO: 'SIb 1',digitacionSIb: '?',tipo: 'Bb2',frecuencia: 116.5}</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
       <c r="A27" s="7">
         <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D27" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E27" t="str">
-        <f>CONCATENATE("var ",C27,"=",D27,";")</f>
+      <c r="F27" t="str">
+        <f t="shared" si="0"/>
         <v>var B2=123.5;</v>
       </c>
-      <c r="F27" t="str">
-        <f>CONCATENATE("case '",C27,"': frequency= ",D27,";break;",)</f>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
         <v>case 'B2': frequency= 123.5;break;</v>
       </c>
-      <c r="G27" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 26,palabra: 'SI 2',tipo: 'B2',frecuencia: 123.5}</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H27" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 26,digitacionDO: 'SI 2',digitacionSIb: '?',tipo: 'B2',frecuencia: 123.5}</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1">
       <c r="A28" s="7">
         <v>27</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E28" t="str">
-        <f>CONCATENATE("var ",C28,"=",D28,";")</f>
+      <c r="F28" t="str">
+        <f t="shared" si="0"/>
         <v>var C3=130.8;</v>
       </c>
-      <c r="F28" t="str">
-        <f>CONCATENATE("case '",C28,"': frequency= ",D28,";break;",)</f>
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
         <v>case 'C3': frequency= 130.8;break;</v>
       </c>
-      <c r="G28" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 27,palabra: 'DO 0',tipo: 'C3',frecuencia: 130.8}</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 27,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C3',frecuencia: 130.8}</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1">
       <c r="A29" s="7">
         <v>28</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C29" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E29" t="str">
-        <f>CONCATENATE("var ",C29,"=",D29,";")</f>
+      <c r="F29" t="str">
+        <f t="shared" si="0"/>
         <v>var Cs3=138.6;</v>
       </c>
-      <c r="F29" t="str">
-        <f>CONCATENATE("case '",C29,"': frequency= ",D29,";break;",)</f>
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Cs3': frequency= 138.6;break;</v>
       </c>
-      <c r="G29" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 28,palabra: 'DO#',tipo: 'Cs3',frecuencia: 138.6}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H29" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 28,digitacionDO: 'DO#',digitacionSIb: '?',tipo: 'Cs3',frecuencia: 138.6}</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1">
       <c r="A30" s="7">
         <v>29</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C30" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E30" t="str">
-        <f>CONCATENATE("var ",C30,"=",D30,";")</f>
+      <c r="F30" t="str">
+        <f t="shared" si="0"/>
         <v>var D3=146.8;</v>
       </c>
-      <c r="F30" t="str">
-        <f>CONCATENATE("case '",C30,"': frequency= ",D30,";break;",)</f>
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
         <v>case 'D3': frequency= 146.8;break;</v>
       </c>
-      <c r="G30" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 29,palabra: 'RE',tipo: 'D3',frecuencia: 146.8}</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H30" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 29,digitacionDO: 'RE',digitacionSIb: '?',tipo: 'D3',frecuencia: 146.8}</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1">
       <c r="A31" s="7">
         <v>30</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E31" t="str">
-        <f>CONCATENATE("var ",C31,"=",D31,";")</f>
+      <c r="F31" t="str">
+        <f t="shared" si="0"/>
         <v>var Eb3=155.6;</v>
       </c>
-      <c r="F31" t="str">
-        <f>CONCATENATE("case '",C31,"': frequency= ",D31,";break;",)</f>
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
         <v>case 'Eb3': frequency= 155.6;break;</v>
       </c>
-      <c r="G31" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 30,palabra: 'Eb3',tipo: 'Eb3',frecuencia: 155.6}</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H31" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 30,digitacionDO: 'Eb3',digitacionSIb: '?',tipo: 'Eb3',frecuencia: 155.6}</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1">
       <c r="A32" s="7">
         <v>31</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C32" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E32" t="str">
-        <f>CONCATENATE("var ",C32,"=",D32,";")</f>
+      <c r="F32" t="str">
+        <f t="shared" si="0"/>
         <v>var E3=164.8;</v>
       </c>
-      <c r="F32" t="str">
-        <f>CONCATENATE("case '",C32,"': frequency= ",D32,";break;",)</f>
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
         <v>case 'E3': frequency= 164.8;break;</v>
       </c>
-      <c r="G32" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 31,palabra: 'MI  1-2',tipo: 'E3',frecuencia: 164.8}</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H32" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 31,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E3',frecuencia: 164.8}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1">
       <c r="A33" s="7">
         <v>32</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E33" t="str">
-        <f>CONCATENATE("var ",C33,"=",D33,";")</f>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
         <v>var F3=174.6;</v>
       </c>
-      <c r="F33" t="str">
-        <f>CONCATENATE("case '",C33,"': frequency= ",D33,";break;",)</f>
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
         <v>case 'F3': frequency= 174.6;break;</v>
       </c>
-      <c r="G33" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 32,palabra: 'F3',tipo: 'F3',frecuencia: 174.6}</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H33" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 32,digitacionDO: 'F3',digitacionSIb: '?',tipo: 'F3',frecuencia: 174.6}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1">
       <c r="A34" s="7">
         <v>33</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E34" t="str">
-        <f>CONCATENATE("var ",C34,"=",D34,";")</f>
+      <c r="F34" t="str">
+        <f t="shared" ref="F34:F65" si="3">CONCATENATE("var ",D34,"=",E34,";")</f>
         <v>var Fs3=185.0;</v>
       </c>
-      <c r="F34" t="str">
-        <f>CONCATENATE("case '",C34,"': frequency= ",D34,";break;",)</f>
+      <c r="G34" t="str">
+        <f t="shared" ref="G34:G64" si="4">CONCATENATE("case '",D34,"': frequency= ",E34,";break;",)</f>
         <v>case 'Fs3': frequency= 185.0;break;</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 33,palabra: 'F#3',tipo: 'Fs3',frecuencia: 185.0}</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H34" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 33,digitacionDO: 'F#3',digitacionSIb: '?',tipo: 'Fs3',frecuencia: 185.0}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1">
       <c r="A35" s="7">
         <v>34</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C35" s="15" t="s">
+      <c r="C35" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E35" t="str">
-        <f>CONCATENATE("var ",C35,"=",D35,";")</f>
+      <c r="F35" t="str">
+        <f t="shared" si="3"/>
         <v>var G3=196.0;</v>
       </c>
-      <c r="F35" t="str">
-        <f>CONCATENATE("case '",C35,"': frequency= ",D35,";break;",)</f>
+      <c r="G35" t="str">
+        <f t="shared" si="4"/>
         <v>case 'G3': frequency= 196.0;break;</v>
       </c>
-      <c r="G35" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 34,palabra: 'G3',tipo: 'G3',frecuencia: 196.0}</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H35" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 34,digitacionDO: 'G3',digitacionSIb: '?',tipo: 'G3',frecuencia: 196.0}</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1">
       <c r="A36" s="7">
         <v>35</v>
       </c>
       <c r="B36" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E36" t="str">
-        <f>CONCATENATE("var ",C36,"=",D36,";")</f>
+      <c r="F36" t="str">
+        <f t="shared" si="3"/>
         <v>var Gs3=207.7;</v>
       </c>
-      <c r="F36" t="str">
-        <f>CONCATENATE("case '",C36,"': frequency= ",D36,";break;",)</f>
+      <c r="G36" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Gs3': frequency= 207.7;break;</v>
       </c>
-      <c r="G36" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 35,palabra: 'G#3',tipo: 'Gs3',frecuencia: 207.7}</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H36" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 35,digitacionDO: 'G#3',digitacionSIb: '?',tipo: 'Gs3',frecuencia: 207.7}</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1">
       <c r="A37" s="7">
         <v>36</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E37" t="str">
-        <f>CONCATENATE("var ",C37,"=",D37,";")</f>
+      <c r="F37" t="str">
+        <f t="shared" si="3"/>
         <v>var A3=220.0;</v>
       </c>
-      <c r="F37" t="str">
-        <f>CONCATENATE("case '",C37,"': frequency= ",D37,";break;",)</f>
+      <c r="G37" t="str">
+        <f t="shared" si="4"/>
         <v>case 'A3': frequency= 220.0;break;</v>
       </c>
-      <c r="G37" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 36,palabra: 'A3',tipo: 'A3',frecuencia: 220.0}</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H37" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 36,digitacionDO: 'A3',digitacionSIb: '?',tipo: 'A3',frecuencia: 220.0}</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1">
       <c r="A38" s="7">
         <v>37</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D38" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E38" t="str">
-        <f>CONCATENATE("var ",C38,"=",D38,";")</f>
+      <c r="F38" t="str">
+        <f t="shared" si="3"/>
         <v>var Bb3=233.1;</v>
       </c>
-      <c r="F38" t="str">
-        <f>CONCATENATE("case '",C38,"': frequency= ",D38,";break;",)</f>
+      <c r="G38" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Bb3': frequency= 233.1;break;</v>
       </c>
-      <c r="G38" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 37,palabra: 'Bb3',tipo: 'Bb3',frecuencia: 233.1}</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H38" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 37,digitacionDO: 'Bb3',digitacionSIb: '?',tipo: 'Bb3',frecuencia: 233.1}</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1">
       <c r="A39" s="7">
         <v>38</v>
       </c>
       <c r="B39" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E39" t="str">
-        <f>CONCATENATE("var ",C39,"=",D39,";")</f>
+      <c r="F39" t="str">
+        <f t="shared" si="3"/>
         <v>var B3=246.9;</v>
       </c>
-      <c r="F39" t="str">
-        <f>CONCATENATE("case '",C39,"': frequency= ",D39,";break;",)</f>
+      <c r="G39" t="str">
+        <f t="shared" si="4"/>
         <v>case 'B3': frequency= 246.9;break;</v>
       </c>
-      <c r="G39" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 38,palabra: 'B3',tipo: 'B3',frecuencia: 246.9}</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H39" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 38,digitacionDO: 'B3',digitacionSIb: '?',tipo: 'B3',frecuencia: 246.9}</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1">
       <c r="A40" s="7">
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E40" t="str">
-        <f>CONCATENATE("var ",C40,"=",D40,";")</f>
+      <c r="F40" t="str">
+        <f t="shared" si="3"/>
         <v>var C4=261.6;</v>
       </c>
-      <c r="F40" t="str">
-        <f>CONCATENATE("case '",C40,"': frequency= ",D40,";break;",)</f>
+      <c r="G40" t="str">
+        <f t="shared" si="4"/>
         <v>case 'C4': frequency= 261.6;break;</v>
       </c>
-      <c r="G40" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 39,palabra: 'C4',tipo: 'C4',frecuencia: 261.6}</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H40" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 39,digitacionDO: 'C4',digitacionSIb: '?',tipo: 'C4',frecuencia: 261.6}</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1">
       <c r="A41" s="7">
         <v>40</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E41" t="str">
-        <f>CONCATENATE("var ",C41,"=",D41,";")</f>
+      <c r="F41" t="str">
+        <f t="shared" si="3"/>
         <v>var Cs4=277.2;</v>
       </c>
-      <c r="F41" t="str">
-        <f>CONCATENATE("case '",C41,"': frequency= ",D41,";break;",)</f>
+      <c r="G41" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Cs4': frequency= 277.2;break;</v>
       </c>
-      <c r="G41" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 40,palabra: 'C#4',tipo: 'Cs4',frecuencia: 277.2}</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H41" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 40,digitacionDO: 'C#4',digitacionSIb: '?',tipo: 'Cs4',frecuencia: 277.2}</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1">
       <c r="A42" s="7">
         <v>41</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E42" t="str">
-        <f>CONCATENATE("var ",C42,"=",D42,";")</f>
+      <c r="F42" t="str">
+        <f t="shared" si="3"/>
         <v>var D4=293.7;</v>
       </c>
-      <c r="F42" t="str">
-        <f>CONCATENATE("case '",C42,"': frequency= ",D42,";break;",)</f>
+      <c r="G42" t="str">
+        <f t="shared" si="4"/>
         <v>case 'D4': frequency= 293.7;break;</v>
       </c>
-      <c r="G42" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 41,palabra: 'D4',tipo: 'D4',frecuencia: 293.7}</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H42" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 41,digitacionDO: 'D4',digitacionSIb: '?',tipo: 'D4',frecuencia: 293.7}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1">
       <c r="A43" s="7">
         <v>42</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E43" t="str">
-        <f>CONCATENATE("var ",C43,"=",D43,";")</f>
+      <c r="F43" t="str">
+        <f t="shared" si="3"/>
         <v>var Eb4=311.1;</v>
       </c>
-      <c r="F43" t="str">
-        <f>CONCATENATE("case '",C43,"': frequency= ",D43,";break;",)</f>
+      <c r="G43" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Eb4': frequency= 311.1;break;</v>
       </c>
-      <c r="G43" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 42,palabra: 'Eb4',tipo: 'Eb4',frecuencia: 311.1}</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H43" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 42,digitacionDO: 'Eb4',digitacionSIb: '?',tipo: 'Eb4',frecuencia: 311.1}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1">
       <c r="A44" s="7">
         <v>43</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C44" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E44" t="str">
-        <f>CONCATENATE("var ",C44,"=",D44,";")</f>
+      <c r="F44" t="str">
+        <f t="shared" si="3"/>
         <v>var E4=329.6;</v>
       </c>
-      <c r="F44" t="str">
-        <f>CONCATENATE("case '",C44,"': frequency= ",D44,";break;",)</f>
+      <c r="G44" t="str">
+        <f t="shared" si="4"/>
         <v>case 'E4': frequency= 329.6;break;</v>
       </c>
-      <c r="G44" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 43,palabra: 'MI  1-2',tipo: 'E4',frecuencia: 329.6}</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H44" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 43,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E4',frecuencia: 329.6}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1">
       <c r="A45" s="7">
         <v>44</v>
       </c>
       <c r="B45" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D45" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E45" t="str">
-        <f>CONCATENATE("var ",C45,"=",D45,";")</f>
+      <c r="F45" t="str">
+        <f t="shared" si="3"/>
         <v>var F4=349.2;</v>
       </c>
-      <c r="F45" t="str">
-        <f>CONCATENATE("case '",C45,"': frequency= ",D45,";break;",)</f>
+      <c r="G45" t="str">
+        <f t="shared" si="4"/>
         <v>case 'F4': frequency= 349.2;break;</v>
       </c>
-      <c r="G45" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 44,palabra: 'F4',tipo: 'F4',frecuencia: 349.2}</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H45" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 44,digitacionDO: 'F4',digitacionSIb: '?',tipo: 'F4',frecuencia: 349.2}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1">
       <c r="A46" s="7">
         <v>45</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E46" t="str">
-        <f>CONCATENATE("var ",C46,"=",D46,";")</f>
+      <c r="F46" t="str">
+        <f t="shared" si="3"/>
         <v>var Fs4=370.0;</v>
       </c>
-      <c r="F46" t="str">
-        <f>CONCATENATE("case '",C46,"': frequency= ",D46,";break;",)</f>
+      <c r="G46" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Fs4': frequency= 370.0;break;</v>
       </c>
-      <c r="G46" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 45,palabra: 'F#4',tipo: 'Fs4',frecuencia: 370.0}</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H46" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 45,digitacionDO: 'F#4',digitacionSIb: '?',tipo: 'Fs4',frecuencia: 370.0}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1">
       <c r="A47" s="7">
         <v>46</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E47" t="str">
-        <f>CONCATENATE("var ",C47,"=",D47,";")</f>
+      <c r="F47" t="str">
+        <f t="shared" si="3"/>
         <v>var G4=392.0;</v>
       </c>
-      <c r="F47" t="str">
-        <f>CONCATENATE("case '",C47,"': frequency= ",D47,";break;",)</f>
+      <c r="G47" t="str">
+        <f t="shared" si="4"/>
         <v>case 'G4': frequency= 392.0;break;</v>
       </c>
-      <c r="G47" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 46,palabra: 'G4',tipo: 'G4',frecuencia: 392.0}</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H47" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 46,digitacionDO: 'G4',digitacionSIb: '?',tipo: 'G4',frecuencia: 392.0}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1">
       <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D48" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E48" t="str">
-        <f>CONCATENATE("var ",C48,"=",D48,";")</f>
+      <c r="F48" t="str">
+        <f t="shared" si="3"/>
         <v>var Gs4=415.3;</v>
       </c>
-      <c r="F48" t="str">
-        <f>CONCATENATE("case '",C48,"': frequency= ",D48,";break;",)</f>
+      <c r="G48" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Gs4': frequency= 415.3;break;</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 47,palabra: 'G#4',tipo: 'Gs4',frecuencia: 415.3}</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H48" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 47,digitacionDO: 'G#4',digitacionSIb: '?',tipo: 'Gs4',frecuencia: 415.3}</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1">
       <c r="A49" s="7">
         <v>48</v>
       </c>
       <c r="B49" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C49" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E49" t="str">
-        <f>CONCATENATE("var ",C49,"=",D49,";")</f>
+      <c r="F49" t="str">
+        <f t="shared" si="3"/>
         <v>var A4=440.0;</v>
       </c>
-      <c r="F49" t="str">
-        <f>CONCATENATE("case '",C49,"': frequency= ",D49,";break;",)</f>
+      <c r="G49" t="str">
+        <f t="shared" si="4"/>
         <v>case 'A4': frequency= 440.0;break;</v>
       </c>
-      <c r="G49" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 48,palabra: 'A4',tipo: 'A4',frecuencia: 440.0}</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H49" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 48,digitacionDO: 'A4',digitacionSIb: '?',tipo: 'A4',frecuencia: 440.0}</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1">
       <c r="A50" s="7">
         <v>49</v>
       </c>
       <c r="B50" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E50" t="str">
-        <f>CONCATENATE("var ",C50,"=",D50,";")</f>
+      <c r="F50" t="str">
+        <f t="shared" si="3"/>
         <v>var Bb4=466.2;</v>
       </c>
-      <c r="F50" t="str">
-        <f>CONCATENATE("case '",C50,"': frequency= ",D50,";break;",)</f>
+      <c r="G50" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Bb4': frequency= 466.2;break;</v>
       </c>
-      <c r="G50" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 49,palabra: 'Bb4',tipo: 'Bb4',frecuencia: 466.2}</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H50" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 49,digitacionDO: 'Bb4',digitacionSIb: '?',tipo: 'Bb4',frecuencia: 466.2}</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1">
       <c r="A51" s="7">
         <v>50</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C51" s="15" t="s">
+      <c r="C51" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E51" t="str">
-        <f>CONCATENATE("var ",C51,"=",D51,";")</f>
+      <c r="F51" t="str">
+        <f t="shared" si="3"/>
         <v>var B4=493.9;</v>
       </c>
-      <c r="F51" t="str">
-        <f>CONCATENATE("case '",C51,"': frequency= ",D51,";break;",)</f>
+      <c r="G51" t="str">
+        <f t="shared" si="4"/>
         <v>case 'B4': frequency= 493.9;break;</v>
       </c>
-      <c r="G51" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 50,palabra: 'B4',tipo: 'B4',frecuencia: 493.9}</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H51" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 50,digitacionDO: 'B4',digitacionSIb: '?',tipo: 'B4',frecuencia: 493.9}</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15.75" thickBot="1">
       <c r="A52" s="7">
         <v>51</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D52" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E52" t="str">
-        <f>CONCATENATE("var ",C52,"=",D52,";")</f>
+      <c r="F52" t="str">
+        <f t="shared" si="3"/>
         <v>var C5=523.3;</v>
       </c>
-      <c r="F52" t="str">
-        <f>CONCATENATE("case '",C52,"': frequency= ",D52,";break;",)</f>
+      <c r="G52" t="str">
+        <f t="shared" si="4"/>
         <v>case 'C5': frequency= 523.3;break;</v>
       </c>
-      <c r="G52" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 51,palabra: 'C5',tipo: 'C5',frecuencia: 523.3}</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H52" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 51,digitacionDO: 'C5',digitacionSIb: '?',tipo: 'C5',frecuencia: 523.3}</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15.75" thickBot="1">
       <c r="A53" s="7">
         <v>52</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E53" t="str">
-        <f>CONCATENATE("var ",C53,"=",D53,";")</f>
+      <c r="F53" t="str">
+        <f t="shared" si="3"/>
         <v>var Cs5=554.4;</v>
       </c>
-      <c r="F53" t="str">
-        <f>CONCATENATE("case '",C53,"': frequency= ",D53,";break;",)</f>
+      <c r="G53" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Cs5': frequency= 554.4;break;</v>
       </c>
-      <c r="G53" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 52,palabra: 'C#5',tipo: 'Cs5',frecuencia: 554.4}</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H53" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 52,digitacionDO: 'C#5',digitacionSIb: '?',tipo: 'Cs5',frecuencia: 554.4}</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15.75" thickBot="1">
       <c r="A54" s="7">
         <v>53</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E54" t="str">
-        <f>CONCATENATE("var ",C54,"=",D54,";")</f>
+      <c r="F54" t="str">
+        <f t="shared" si="3"/>
         <v>var D5=587.3;</v>
       </c>
-      <c r="F54" t="str">
-        <f>CONCATENATE("case '",C54,"': frequency= ",D54,";break;",)</f>
+      <c r="G54" t="str">
+        <f t="shared" si="4"/>
         <v>case 'D5': frequency= 587.3;break;</v>
       </c>
-      <c r="G54" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 53,palabra: 'D5',tipo: 'D5',frecuencia: 587.3}</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H54" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 53,digitacionDO: 'D5',digitacionSIb: '?',tipo: 'D5',frecuencia: 587.3}</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15.75" thickBot="1">
       <c r="A55" s="7">
         <v>54</v>
       </c>
       <c r="B55" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="15" t="s">
+      <c r="C55" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D55" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E55" t="str">
-        <f>CONCATENATE("var ",C55,"=",D55,";")</f>
+      <c r="F55" t="str">
+        <f t="shared" si="3"/>
         <v>var Eb5=622.3;</v>
       </c>
-      <c r="F55" t="str">
-        <f>CONCATENATE("case '",C55,"': frequency= ",D55,";break;",)</f>
+      <c r="G55" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Eb5': frequency= 622.3;break;</v>
       </c>
-      <c r="G55" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 54,palabra: 'Eb5',tipo: 'Eb5',frecuencia: 622.3}</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H55" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 54,digitacionDO: 'Eb5',digitacionSIb: '?',tipo: 'Eb5',frecuencia: 622.3}</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.75" thickBot="1">
       <c r="A56" s="7">
         <v>55</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="C56" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="D56" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="E56" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E56" t="str">
-        <f>CONCATENATE("var ",C56,"=",D56,";")</f>
+      <c r="F56" t="str">
+        <f t="shared" si="3"/>
         <v>var E5=659.3;</v>
       </c>
-      <c r="F56" t="str">
-        <f>CONCATENATE("case '",C56,"': frequency= ",D56,";break;",)</f>
+      <c r="G56" t="str">
+        <f t="shared" si="4"/>
         <v>case 'E5': frequency= 659.3;break;</v>
       </c>
-      <c r="G56" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 55,palabra: 'MI  1-2',tipo: 'E5',frecuencia: 659.3}</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H56" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 55,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E5',frecuencia: 659.3}</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" thickBot="1">
       <c r="A57" s="7">
         <v>56</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="15" t="s">
+      <c r="C57" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D57" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="2" t="s">
+      <c r="E57" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E57" t="str">
-        <f>CONCATENATE("var ",C57,"=",D57,";")</f>
+      <c r="F57" t="str">
+        <f t="shared" si="3"/>
         <v>var F5=698.5;</v>
       </c>
-      <c r="F57" t="str">
-        <f>CONCATENATE("case '",C57,"': frequency= ",D57,";break;",)</f>
+      <c r="G57" t="str">
+        <f t="shared" si="4"/>
         <v>case 'F5': frequency= 698.5;break;</v>
       </c>
-      <c r="G57" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 56,palabra: 'F5',tipo: 'F5',frecuencia: 698.5}</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H57" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 56,digitacionDO: 'F5',digitacionSIb: '?',tipo: 'F5',frecuencia: 698.5}</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15.75" thickBot="1">
       <c r="A58" s="7">
         <v>57</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="15" t="s">
+      <c r="C58" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E58" t="str">
-        <f>CONCATENATE("var ",C58,"=",D58,";")</f>
+      <c r="F58" t="str">
+        <f t="shared" si="3"/>
         <v>var Fs5=740.0;</v>
       </c>
-      <c r="F58" t="str">
-        <f>CONCATENATE("case '",C58,"': frequency= ",D58,";break;",)</f>
+      <c r="G58" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Fs5': frequency= 740.0;break;</v>
       </c>
-      <c r="G58" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 57,palabra: 'F#5',tipo: 'Fs5',frecuencia: 740.0}</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H58" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 57,digitacionDO: 'F#5',digitacionSIb: '?',tipo: 'Fs5',frecuencia: 740.0}</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" thickBot="1">
       <c r="A59" s="7">
         <v>58</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="C59" s="15" t="s">
+      <c r="C59" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D59" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E59" t="str">
-        <f>CONCATENATE("var ",C59,"=",D59,";")</f>
+      <c r="F59" t="str">
+        <f t="shared" si="3"/>
         <v>var G5=784.0;</v>
       </c>
-      <c r="F59" t="str">
-        <f>CONCATENATE("case '",C59,"': frequency= ",D59,";break;",)</f>
+      <c r="G59" t="str">
+        <f t="shared" si="4"/>
         <v>case 'G5': frequency= 784.0;break;</v>
       </c>
-      <c r="G59" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 58,palabra: 'G5',tipo: 'G5',frecuencia: 784.0}</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 58,digitacionDO: 'G5',digitacionSIb: '?',tipo: 'G5',frecuencia: 784.0}</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15.75" thickBot="1">
       <c r="A60" s="7">
         <v>59</v>
       </c>
       <c r="B60" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D60" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E60" t="str">
-        <f>CONCATENATE("var ",C60,"=",D60,";")</f>
+      <c r="F60" t="str">
+        <f t="shared" si="3"/>
         <v>var Gs5=830.6;</v>
       </c>
-      <c r="F60" t="str">
-        <f>CONCATENATE("case '",C60,"': frequency= ",D60,";break;",)</f>
+      <c r="G60" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Gs5': frequency= 830.6;break;</v>
       </c>
-      <c r="G60" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 59,palabra: 'G#5',tipo: 'Gs5',frecuencia: 830.6}</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 59,digitacionDO: 'G#5',digitacionSIb: '?',tipo: 'Gs5',frecuencia: 830.6}</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="15.75" thickBot="1">
       <c r="A61" s="7">
         <v>60</v>
       </c>
       <c r="B61" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E61" t="str">
-        <f>CONCATENATE("var ",C61,"=",D61,";")</f>
+      <c r="F61" t="str">
+        <f t="shared" si="3"/>
         <v>var A5=880.0;</v>
       </c>
-      <c r="F61" t="str">
-        <f>CONCATENATE("case '",C61,"': frequency= ",D61,";break;",)</f>
+      <c r="G61" t="str">
+        <f t="shared" si="4"/>
         <v>case 'A5': frequency= 880.0;break;</v>
       </c>
-      <c r="G61" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 60,palabra: 'A5',tipo: 'A5',frecuencia: 880.0}</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 60,digitacionDO: 'A5',digitacionSIb: '?',tipo: 'A5',frecuencia: 880.0}</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" thickBot="1">
       <c r="A62" s="7">
         <v>61</v>
       </c>
       <c r="B62" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="2" t="s">
+      <c r="E62" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E62" t="str">
-        <f>CONCATENATE("var ",C62,"=",D62,";")</f>
+      <c r="F62" t="str">
+        <f t="shared" si="3"/>
         <v>var Bb5=932.3;</v>
       </c>
-      <c r="F62" t="str">
-        <f>CONCATENATE("case '",C62,"': frequency= ",D62,";break;",)</f>
+      <c r="G62" t="str">
+        <f t="shared" si="4"/>
         <v>case 'Bb5': frequency= 932.3;break;</v>
       </c>
-      <c r="G62" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 61,palabra: 'Bb5',tipo: 'Bb5',frecuencia: 932.3}</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 61,digitacionDO: 'Bb5',digitacionSIb: '?',tipo: 'Bb5',frecuencia: 932.3}</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" thickBot="1">
       <c r="A63" s="7">
         <v>62</v>
       </c>
       <c r="B63" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D63" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E63" t="str">
-        <f>CONCATENATE("var ",C63,"=",D63,";")</f>
+      <c r="F63" t="str">
+        <f t="shared" si="3"/>
         <v>var B5=987.8;</v>
       </c>
-      <c r="F63" t="str">
-        <f>CONCATENATE("case '",C63,"': frequency= ",D63,";break;",)</f>
+      <c r="G63" t="str">
+        <f t="shared" si="4"/>
         <v>case 'B5': frequency= 987.8;break;</v>
       </c>
-      <c r="G63" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 62,palabra: 'B5',tipo: 'B5',frecuencia: 987.8}</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="15.75" thickBot="1">
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 62,digitacionDO: 'B5',digitacionSIb: '?',tipo: 'B5',frecuencia: 987.8}</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="15.75" thickBot="1">
       <c r="A64" s="7">
         <v>63</v>
       </c>
       <c r="B64" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D64" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="2">
+      <c r="E64" s="2">
         <v>1047</v>
       </c>
-      <c r="E64" t="str">
-        <f>CONCATENATE("var ",C64,"=",D64,";")</f>
+      <c r="F64" t="str">
+        <f t="shared" si="3"/>
         <v>var C6=1047;</v>
       </c>
-      <c r="F64" t="str">
-        <f>CONCATENATE("case '",C64,"': frequency= ",D64,";break;",)</f>
+      <c r="G64" t="str">
+        <f t="shared" si="4"/>
         <v>case 'C6': frequency= 1047;break;</v>
       </c>
-      <c r="G64" t="str">
-        <f t="shared" si="0"/>
-        <v>{indice: 63,palabra: 'C6',tipo: 'C6',frecuencia: 1047}</v>
-      </c>
-    </row>
-    <row r="65" spans="2:69" ht="15.75" thickBot="1">
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>{indice: 63,digitacionDO: 'C6',digitacionSIb: '?',tipo: 'C6',frecuencia: 1047}</v>
+      </c>
+    </row>
+    <row r="65" spans="2:70" ht="15.75" thickBot="1">
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
-    </row>
-    <row r="66" spans="2:69" ht="15.75" thickBot="1">
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="2:70" ht="15.75" thickBot="1">
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="G66" t="str" cm="1">
-        <f t="array" ref="G66:BQ66">CONCATENATE(TRANSPOSE(G2:G64)&amp;",")</f>
-        <v>{indice: 1,palabra: 'DO 0',tipo: 'C1',frecuencia: 32.70},</v>
-      </c>
-      <c r="H66" t="str">
-        <v>{indice: 2,palabra: 'C#1',tipo: 'Cs1',frecuencia: 34.65},</v>
+      <c r="E66" s="1"/>
+      <c r="H66" t="str" cm="1">
+        <f t="array" ref="H66:BR66">CONCATENATE(TRANSPOSE(H2:H64)&amp;",")</f>
+        <v>{indice: 1,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C1',frecuencia: 32.70},</v>
       </c>
       <c r="I66" t="str">
-        <v>{indice: 3,palabra: 'D1',tipo: 'D1',frecuencia: 36.71},</v>
+        <v>{indice: 2,digitacionDO: 'C#1',digitacionSIb: '?',tipo: 'Cs1',frecuencia: 34.65},</v>
       </c>
       <c r="J66" t="str">
-        <v>{indice: 4,palabra: 'Eb1',tipo: 'Eb1',frecuencia: 38.89},</v>
+        <v>{indice: 3,digitacionDO: 'D1',digitacionSIb: '?',tipo: 'D1',frecuencia: 36.71},</v>
       </c>
       <c r="K66" t="str">
-        <v>{indice: 5,palabra: 'E1',tipo: 'E1',frecuencia: 41.20},</v>
+        <v>{indice: 4,digitacionDO: 'Eb1',digitacionSIb: '?',tipo: 'Eb1',frecuencia: 38.89},</v>
       </c>
       <c r="L66" t="str">
-        <v>{indice: 6,palabra: 'F1',tipo: 'F1',frecuencia: 43.65},</v>
+        <v>{indice: 5,digitacionDO: 'E1',digitacionSIb: '?',tipo: 'E1',frecuencia: 41.20},</v>
       </c>
       <c r="M66" t="str">
-        <v>{indice: 7,palabra: 'F#1',tipo: 'Fs1',frecuencia: 46.25},</v>
+        <v>{indice: 6,digitacionDO: 'F1',digitacionSIb: '?',tipo: 'F1',frecuencia: 43.65},</v>
       </c>
       <c r="N66" t="str">
-        <v>{indice: 8,palabra: 'G1',tipo: 'G1',frecuencia: 49.00},</v>
+        <v>{indice: 7,digitacionDO: 'F#1',digitacionSIb: '?',tipo: 'Fs1',frecuencia: 46.25},</v>
       </c>
       <c r="O66" t="str">
-        <v>{indice: 9,palabra: 'G#1',tipo: 'Gs1',frecuencia: 51.91},</v>
+        <v>{indice: 8,digitacionDO: 'G1',digitacionSIb: '?',tipo: 'G1',frecuencia: 49.00},</v>
       </c>
       <c r="P66" t="str">
-        <v>{indice: 10,palabra: 'LA 1-2',tipo: 'A1',frecuencia: 55.00},</v>
+        <v>{indice: 9,digitacionDO: 'G#1',digitacionSIb: '?',tipo: 'Gs1',frecuencia: 51.91},</v>
       </c>
       <c r="Q66" t="str">
-        <v>{indice: 11,palabra: 'SIb 1',tipo: 'Bb1',frecuencia: 58.27},</v>
+        <v>{indice: 10,digitacionDO: 'LA 1-2',digitacionSIb: '?',tipo: 'A1',frecuencia: 55.00},</v>
       </c>
       <c r="R66" t="str">
-        <v>{indice: 12,palabra: 'SI 2',tipo: 'B1',frecuencia: 61.74},</v>
+        <v>{indice: 11,digitacionDO: 'SIb 1',digitacionSIb: '?',tipo: 'Bb1',frecuencia: 58.27},</v>
       </c>
       <c r="S66" t="str">
-        <v>{indice: 13,palabra: 'DO 0',tipo: 'C2',frecuencia: 65.41},</v>
+        <v>{indice: 12,digitacionDO: 'SI 2',digitacionSIb: '?',tipo: 'B1',frecuencia: 61.74},</v>
       </c>
       <c r="T66" t="str">
-        <v>{indice: 14,palabra: 'DO#',tipo: 'Cs2',frecuencia: 69.30},</v>
+        <v>{indice: 13,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C2',frecuencia: 65.41},</v>
       </c>
       <c r="U66" t="str">
-        <v>{indice: 15,palabra: 'RE b',tipo: 'Db2',frecuencia: 69.30},</v>
+        <v>{indice: 14,digitacionDO: 'DO#',digitacionSIb: '?',tipo: 'Cs2',frecuencia: 69.30},</v>
       </c>
       <c r="V66" t="str">
-        <v>{indice: 16,palabra: 'RE',tipo: 'D2',frecuencia: 73.42},</v>
+        <v>{indice: 15,digitacionDO: 'RE b',digitacionSIb: '?',tipo: 'Db2',frecuencia: 69.30},</v>
       </c>
       <c r="W66" t="str">
-        <v>{indice: 17,palabra: 'RE#',tipo: 'Ds2',frecuencia: 77.78},</v>
+        <v>{indice: 16,digitacionDO: 'RE',digitacionSIb: '?',tipo: 'D2',frecuencia: 73.42},</v>
       </c>
       <c r="X66" t="str">
-        <v>{indice: 18,palabra: 'MI b',tipo: 'Eb2',frecuencia: 77.78},</v>
+        <v>{indice: 17,digitacionDO: 'RE#',digitacionSIb: '?',tipo: 'Ds2',frecuencia: 77.78},</v>
       </c>
       <c r="Y66" t="str">
-        <v>{indice: 19,palabra: 'MI  1-2',tipo: 'E2',frecuencia: 82.41},</v>
+        <v>{indice: 18,digitacionDO: 'MI b',digitacionSIb: '?',tipo: 'Eb2',frecuencia: 77.78},</v>
       </c>
       <c r="Z66" t="str">
-        <v>{indice: 20,palabra: 'FA 1',tipo: 'F2',frecuencia: 87.31},</v>
+        <v>{indice: 19,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E2',frecuencia: 82.41},</v>
       </c>
       <c r="AA66" t="str">
-        <v>{indice: 21,palabra: 'FA# 2',tipo: 'Fs2',frecuencia: 92.50},</v>
+        <v>{indice: 20,digitacionDO: 'FA 1',digitacionSIb: '?',tipo: 'F2',frecuencia: 87.31},</v>
       </c>
       <c r="AB66" t="str">
-        <v>{indice: 22,palabra: 'SOL 0',tipo: 'G2',frecuencia: 98.00},</v>
+        <v>{indice: 21,digitacionDO: 'FA# 2',digitacionSIb: '?',tipo: 'Fs2',frecuencia: 92.50},</v>
       </c>
       <c r="AC66" t="str">
-        <v>{indice: 23,palabra: 'SOL#',tipo: 'Gs2',frecuencia: 103.8},</v>
+        <v>{indice: 22,digitacionDO: 'SOL 0',digitacionSIb: '?',tipo: 'G2',frecuencia: 98.00},</v>
       </c>
       <c r="AD66" t="str">
-        <v>{indice: 24,palabra: 'LA 1-2',tipo: 'A2',frecuencia: 110.0},</v>
+        <v>{indice: 23,digitacionDO: 'SOL#',digitacionSIb: '?',tipo: 'Gs2',frecuencia: 103.8},</v>
       </c>
       <c r="AE66" t="str">
-        <v>{indice: 25,palabra: 'SIb 1',tipo: 'Bb2',frecuencia: 116.5},</v>
+        <v>{indice: 24,digitacionDO: 'LA 1-2',digitacionSIb: '?',tipo: 'A2',frecuencia: 110.0},</v>
       </c>
       <c r="AF66" t="str">
-        <v>{indice: 26,palabra: 'SI 2',tipo: 'B2',frecuencia: 123.5},</v>
+        <v>{indice: 25,digitacionDO: 'SIb 1',digitacionSIb: '?',tipo: 'Bb2',frecuencia: 116.5},</v>
       </c>
       <c r="AG66" t="str">
-        <v>{indice: 27,palabra: 'DO 0',tipo: 'C3',frecuencia: 130.8},</v>
+        <v>{indice: 26,digitacionDO: 'SI 2',digitacionSIb: '?',tipo: 'B2',frecuencia: 123.5},</v>
       </c>
       <c r="AH66" t="str">
-        <v>{indice: 28,palabra: 'DO#',tipo: 'Cs3',frecuencia: 138.6},</v>
+        <v>{indice: 27,digitacionDO: 'DO 0',digitacionSIb: '?',tipo: 'C3',frecuencia: 130.8},</v>
       </c>
       <c r="AI66" t="str">
-        <v>{indice: 29,palabra: 'RE',tipo: 'D3',frecuencia: 146.8},</v>
+        <v>{indice: 28,digitacionDO: 'DO#',digitacionSIb: '?',tipo: 'Cs3',frecuencia: 138.6},</v>
       </c>
       <c r="AJ66" t="str">
-        <v>{indice: 30,palabra: 'Eb3',tipo: 'Eb3',frecuencia: 155.6},</v>
+        <v>{indice: 29,digitacionDO: 'RE',digitacionSIb: '?',tipo: 'D3',frecuencia: 146.8},</v>
       </c>
       <c r="AK66" t="str">
-        <v>{indice: 31,palabra: 'MI  1-2',tipo: 'E3',frecuencia: 164.8},</v>
+        <v>{indice: 30,digitacionDO: 'Eb3',digitacionSIb: '?',tipo: 'Eb3',frecuencia: 155.6},</v>
       </c>
       <c r="AL66" t="str">
-        <v>{indice: 32,palabra: 'F3',tipo: 'F3',frecuencia: 174.6},</v>
+        <v>{indice: 31,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E3',frecuencia: 164.8},</v>
       </c>
       <c r="AM66" t="str">
-        <v>{indice: 33,palabra: 'F#3',tipo: 'Fs3',frecuencia: 185.0},</v>
+        <v>{indice: 32,digitacionDO: 'F3',digitacionSIb: '?',tipo: 'F3',frecuencia: 174.6},</v>
       </c>
       <c r="AN66" t="str">
-        <v>{indice: 34,palabra: 'G3',tipo: 'G3',frecuencia: 196.0},</v>
+        <v>{indice: 33,digitacionDO: 'F#3',digitacionSIb: '?',tipo: 'Fs3',frecuencia: 185.0},</v>
       </c>
       <c r="AO66" t="str">
-        <v>{indice: 35,palabra: 'G#3',tipo: 'Gs3',frecuencia: 207.7},</v>
+        <v>{indice: 34,digitacionDO: 'G3',digitacionSIb: '?',tipo: 'G3',frecuencia: 196.0},</v>
       </c>
       <c r="AP66" t="str">
-        <v>{indice: 36,palabra: 'A3',tipo: 'A3',frecuencia: 220.0},</v>
+        <v>{indice: 35,digitacionDO: 'G#3',digitacionSIb: '?',tipo: 'Gs3',frecuencia: 207.7},</v>
       </c>
       <c r="AQ66" t="str">
-        <v>{indice: 37,palabra: 'Bb3',tipo: 'Bb3',frecuencia: 233.1},</v>
+        <v>{indice: 36,digitacionDO: 'A3',digitacionSIb: '?',tipo: 'A3',frecuencia: 220.0},</v>
       </c>
       <c r="AR66" t="str">
-        <v>{indice: 38,palabra: 'B3',tipo: 'B3',frecuencia: 246.9},</v>
+        <v>{indice: 37,digitacionDO: 'Bb3',digitacionSIb: '?',tipo: 'Bb3',frecuencia: 233.1},</v>
       </c>
       <c r="AS66" t="str">
-        <v>{indice: 39,palabra: 'C4',tipo: 'C4',frecuencia: 261.6},</v>
+        <v>{indice: 38,digitacionDO: 'B3',digitacionSIb: '?',tipo: 'B3',frecuencia: 246.9},</v>
       </c>
       <c r="AT66" t="str">
-        <v>{indice: 40,palabra: 'C#4',tipo: 'Cs4',frecuencia: 277.2},</v>
+        <v>{indice: 39,digitacionDO: 'C4',digitacionSIb: '?',tipo: 'C4',frecuencia: 261.6},</v>
       </c>
       <c r="AU66" t="str">
-        <v>{indice: 41,palabra: 'D4',tipo: 'D4',frecuencia: 293.7},</v>
+        <v>{indice: 40,digitacionDO: 'C#4',digitacionSIb: '?',tipo: 'Cs4',frecuencia: 277.2},</v>
       </c>
       <c r="AV66" t="str">
-        <v>{indice: 42,palabra: 'Eb4',tipo: 'Eb4',frecuencia: 311.1},</v>
+        <v>{indice: 41,digitacionDO: 'D4',digitacionSIb: '?',tipo: 'D4',frecuencia: 293.7},</v>
       </c>
       <c r="AW66" t="str">
-        <v>{indice: 43,palabra: 'MI  1-2',tipo: 'E4',frecuencia: 329.6},</v>
+        <v>{indice: 42,digitacionDO: 'Eb4',digitacionSIb: '?',tipo: 'Eb4',frecuencia: 311.1},</v>
       </c>
       <c r="AX66" t="str">
-        <v>{indice: 44,palabra: 'F4',tipo: 'F4',frecuencia: 349.2},</v>
+        <v>{indice: 43,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E4',frecuencia: 329.6},</v>
       </c>
       <c r="AY66" t="str">
-        <v>{indice: 45,palabra: 'F#4',tipo: 'Fs4',frecuencia: 370.0},</v>
+        <v>{indice: 44,digitacionDO: 'F4',digitacionSIb: '?',tipo: 'F4',frecuencia: 349.2},</v>
       </c>
       <c r="AZ66" t="str">
-        <v>{indice: 46,palabra: 'G4',tipo: 'G4',frecuencia: 392.0},</v>
+        <v>{indice: 45,digitacionDO: 'F#4',digitacionSIb: '?',tipo: 'Fs4',frecuencia: 370.0},</v>
       </c>
       <c r="BA66" t="str">
-        <v>{indice: 47,palabra: 'G#4',tipo: 'Gs4',frecuencia: 415.3},</v>
+        <v>{indice: 46,digitacionDO: 'G4',digitacionSIb: '?',tipo: 'G4',frecuencia: 392.0},</v>
       </c>
       <c r="BB66" t="str">
-        <v>{indice: 48,palabra: 'A4',tipo: 'A4',frecuencia: 440.0},</v>
+        <v>{indice: 47,digitacionDO: 'G#4',digitacionSIb: '?',tipo: 'Gs4',frecuencia: 415.3},</v>
       </c>
       <c r="BC66" t="str">
-        <v>{indice: 49,palabra: 'Bb4',tipo: 'Bb4',frecuencia: 466.2},</v>
+        <v>{indice: 48,digitacionDO: 'A4',digitacionSIb: '?',tipo: 'A4',frecuencia: 440.0},</v>
       </c>
       <c r="BD66" t="str">
-        <v>{indice: 50,palabra: 'B4',tipo: 'B4',frecuencia: 493.9},</v>
+        <v>{indice: 49,digitacionDO: 'Bb4',digitacionSIb: '?',tipo: 'Bb4',frecuencia: 466.2},</v>
       </c>
       <c r="BE66" t="str">
-        <v>{indice: 51,palabra: 'C5',tipo: 'C5',frecuencia: 523.3},</v>
+        <v>{indice: 50,digitacionDO: 'B4',digitacionSIb: '?',tipo: 'B4',frecuencia: 493.9},</v>
       </c>
       <c r="BF66" t="str">
-        <v>{indice: 52,palabra: 'C#5',tipo: 'Cs5',frecuencia: 554.4},</v>
+        <v>{indice: 51,digitacionDO: 'C5',digitacionSIb: '?',tipo: 'C5',frecuencia: 523.3},</v>
       </c>
       <c r="BG66" t="str">
-        <v>{indice: 53,palabra: 'D5',tipo: 'D5',frecuencia: 587.3},</v>
+        <v>{indice: 52,digitacionDO: 'C#5',digitacionSIb: '?',tipo: 'Cs5',frecuencia: 554.4},</v>
       </c>
       <c r="BH66" t="str">
-        <v>{indice: 54,palabra: 'Eb5',tipo: 'Eb5',frecuencia: 622.3},</v>
+        <v>{indice: 53,digitacionDO: 'D5',digitacionSIb: '?',tipo: 'D5',frecuencia: 587.3},</v>
       </c>
       <c r="BI66" t="str">
-        <v>{indice: 55,palabra: 'MI  1-2',tipo: 'E5',frecuencia: 659.3},</v>
+        <v>{indice: 54,digitacionDO: 'Eb5',digitacionSIb: '?',tipo: 'Eb5',frecuencia: 622.3},</v>
       </c>
       <c r="BJ66" t="str">
-        <v>{indice: 56,palabra: 'F5',tipo: 'F5',frecuencia: 698.5},</v>
+        <v>{indice: 55,digitacionDO: 'MI  1-2',digitacionSIb: '?',tipo: 'E5',frecuencia: 659.3},</v>
       </c>
       <c r="BK66" t="str">
-        <v>{indice: 57,palabra: 'F#5',tipo: 'Fs5',frecuencia: 740.0},</v>
+        <v>{indice: 56,digitacionDO: 'F5',digitacionSIb: '?',tipo: 'F5',frecuencia: 698.5},</v>
       </c>
       <c r="BL66" t="str">
-        <v>{indice: 58,palabra: 'G5',tipo: 'G5',frecuencia: 784.0},</v>
+        <v>{indice: 57,digitacionDO: 'F#5',digitacionSIb: '?',tipo: 'Fs5',frecuencia: 740.0},</v>
       </c>
       <c r="BM66" t="str">
-        <v>{indice: 59,palabra: 'G#5',tipo: 'Gs5',frecuencia: 830.6},</v>
+        <v>{indice: 58,digitacionDO: 'G5',digitacionSIb: '?',tipo: 'G5',frecuencia: 784.0},</v>
       </c>
       <c r="BN66" t="str">
-        <v>{indice: 60,palabra: 'A5',tipo: 'A5',frecuencia: 880.0},</v>
+        <v>{indice: 59,digitacionDO: 'G#5',digitacionSIb: '?',tipo: 'Gs5',frecuencia: 830.6},</v>
       </c>
       <c r="BO66" t="str">
-        <v>{indice: 61,palabra: 'Bb5',tipo: 'Bb5',frecuencia: 932.3},</v>
+        <v>{indice: 60,digitacionDO: 'A5',digitacionSIb: '?',tipo: 'A5',frecuencia: 880.0},</v>
       </c>
       <c r="BP66" t="str">
-        <v>{indice: 62,palabra: 'B5',tipo: 'B5',frecuencia: 987.8},</v>
+        <v>{indice: 61,digitacionDO: 'Bb5',digitacionSIb: '?',tipo: 'Bb5',frecuencia: 932.3},</v>
       </c>
       <c r="BQ66" t="str">
-        <v>{indice: 63,palabra: 'C6',tipo: 'C6',frecuencia: 1047},</v>
+        <v>{indice: 62,digitacionDO: 'B5',digitacionSIb: '?',tipo: 'B5',frecuencia: 987.8},</v>
+      </c>
+      <c r="BR66" t="str">
+        <v>{indice: 63,digitacionDO: 'C6',digitacionSIb: '?',tipo: 'C6',frecuencia: 1047},</v>
       </c>
     </row>
   </sheetData>
@@ -3905,7 +4106,7 @@
         <v>138</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D2:D41" si="0">CONCATENATE("{indice: '",A3,"',palabra: '",B3,"',tipo: '",C3,"'}")</f>
+        <f t="shared" ref="D3:D41" si="0">CONCATENATE("{indice: '",A3,"',palabra: '",B3,"',tipo: '",C3,"'}")</f>
         <v>{indice: '2',palabra: 'LA 1-2',tipo: 'A2'}</v>
       </c>
     </row>

</xml_diff>